<commit_message>
Alterações Disp x Agravo (agora com Suspeita em Aberto e com Atendimento)
</commit_message>
<xml_diff>
--- a/Separa unidades/Unidades/America.xlsx
+++ b/Separa unidades/Unidades/America.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="21">
   <si>
     <t>ID DISP.</t>
   </si>
@@ -34,6 +34,12 @@
     <t>ID. PACIENTE</t>
   </si>
   <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Foi atendido</t>
+  </si>
+  <si>
     <t>19/04/2021</t>
   </si>
   <si>
@@ -52,7 +58,25 @@
     <t>23/06/2021</t>
   </si>
   <si>
+    <t>29/06/2021</t>
+  </si>
+  <si>
+    <t>06/07/2021</t>
+  </si>
+  <si>
     <t>UBS DR MILTON BARONI DE BARRETOS</t>
+  </si>
+  <si>
+    <t>PACIENTE SEM SUSPEITA</t>
+  </si>
+  <si>
+    <t>PACIENTE COM SUSPEITA EM ABERTO</t>
+  </si>
+  <si>
+    <t>NÃO</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
@@ -410,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,19 +459,25 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1872177</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2064081</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -455,19 +485,25 @@
       <c r="F2">
         <v>82440</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1884539</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>2064081</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -475,19 +511,25 @@
       <c r="F3">
         <v>4143</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1897653</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2064081</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -495,19 +537,25 @@
       <c r="F4">
         <v>55440</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1897686</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>2064081</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -515,19 +563,25 @@
       <c r="F5">
         <v>332561</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>1897689</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>2064081</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -535,19 +589,25 @@
       <c r="F6">
         <v>230722</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>1897691</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2064081</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -555,59 +615,77 @@
       <c r="F7">
         <v>46858</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
+        <v>1897696</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>2064081</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>78306</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
         <v>1897693</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>2064081</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2064081</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>95249</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>1897696</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>2064081</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>78306</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>1897703</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>2064081</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -615,19 +693,25 @@
       <c r="F10">
         <v>85991</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>1917669</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>2064081</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -635,19 +719,25 @@
       <c r="F11">
         <v>88102</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1955001</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>2064081</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -655,19 +745,25 @@
       <c r="F12">
         <v>86267</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>1957247</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>2064081</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -675,19 +771,25 @@
       <c r="F13">
         <v>246175</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1958038</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2064081</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -695,25 +797,167 @@
       <c r="F14">
         <v>16325</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>1958036</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>2064081</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
         <v>260075</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>1964304</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2064081</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>226861</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1973147</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>2064081</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>44582</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1972855</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2064081</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>10335</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>1972871</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>2064081</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>77902</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>1973400</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>2064081</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>13337</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>